<commit_message>
edits to fire_spread and dispersion scripts
</commit_message>
<xml_diff>
--- a/RxCADRE/L2G/profile_builder.xlsx
+++ b/RxCADRE/L2G/profile_builder.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24280" yWindow="3240" windowWidth="22660" windowHeight="22240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="24280" yWindow="3240" windowWidth="22660" windowHeight="22240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Adjusted Idealized" sheetId="4" r:id="rId1"/>
+    <sheet name="Unadjusted Real" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_10_11_2012_pre" localSheetId="1">Sheet2!$A$2:$M$188</definedName>
+    <definedName name="_10_11_2012_pre" localSheetId="2">Sheet2!$A$2:$M$188</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Surface Pressure (MB)</t>
   </si>
@@ -173,6 +174,18 @@
   <si>
     <t>Wind speed</t>
   </si>
+  <si>
+    <t>WSPD</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>WDIR</t>
+  </si>
+  <si>
+    <t>SFC AGL</t>
+  </si>
 </sst>
 </file>
 
@@ -243,9 +256,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -285,7 +308,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -301,6 +324,11 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -317,6 +345,11 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -650,10 +683,4849 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K188"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L179" sqref="L179"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1">
+        <f>62</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1020</v>
+      </c>
+      <c r="B2">
+        <v>298</v>
+      </c>
+      <c r="C2">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="3">
+        <f>I7-$K$1</f>
+        <v>-0.1255999999999986</v>
+      </c>
+      <c r="B7" s="3">
+        <v>298.93220776140924</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <f>COS(RADIANS($K$5))*J7</f>
+        <v>-1.2855752193730787</v>
+      </c>
+      <c r="E7" s="5">
+        <f>SIN(RADIANS($K$5))*J7</f>
+        <v>1.532088886237956</v>
+      </c>
+      <c r="I7" s="3">
+        <v>61.874400000000001</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="3">
+        <f t="shared" ref="A8:A71" si="0">I8-$K$1</f>
+        <v>9.0183999999999997</v>
+      </c>
+      <c r="B8" s="3">
+        <v>297.14828178301372</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" ref="D8:D71" si="1">COS(RADIANS($K$5))*J8</f>
+        <v>-1.7355265461536564</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:E71" si="2">SIN(RADIANS($K$5))*J8</f>
+        <v>2.0683199964212409</v>
+      </c>
+      <c r="I8" s="3">
+        <v>71.0184</v>
+      </c>
+      <c r="J8">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>23.039200000000008</v>
+      </c>
+      <c r="B9" s="3">
+        <v>294.10769650274869</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.1854778729342339</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="2"/>
+        <v>2.604551106604525</v>
+      </c>
+      <c r="I9" s="3">
+        <v>85.039200000000008</v>
+      </c>
+      <c r="J9">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>37.974400000000003</v>
+      </c>
+      <c r="B10" s="3">
+        <v>291.06145317374052</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I10" s="3">
+        <v>99.974400000000003</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>51.080800000000011</v>
+      </c>
+      <c r="B11" s="3">
+        <v>290.93704053544832</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I11" s="3">
+        <v>113.08080000000001</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>61.139200000000002</v>
+      </c>
+      <c r="B12" s="3">
+        <v>290.73764340322123</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I12" s="3">
+        <v>123.1392</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3">
+        <f t="shared" si="0"/>
+        <v>73.940799999999996</v>
+      </c>
+      <c r="B13" s="3">
+        <v>290.51330750172093</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I13" s="3">
+        <v>135.9408</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="3">
+        <f t="shared" si="0"/>
+        <v>86.132800000000003</v>
+      </c>
+      <c r="B14" s="3">
+        <v>290.28892563193062</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I14" s="3">
+        <v>148.1328</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="3">
+        <f t="shared" si="0"/>
+        <v>101.06800000000001</v>
+      </c>
+      <c r="B15" s="3">
+        <v>289.84857837420185</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I15" s="3">
+        <v>163.06800000000001</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="3">
+        <f t="shared" si="0"/>
+        <v>112.95520000000002</v>
+      </c>
+      <c r="B16" s="3">
+        <v>289.3253908793904</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I16" s="3">
+        <v>174.95520000000002</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3">
+        <f t="shared" si="0"/>
+        <v>126.0616</v>
+      </c>
+      <c r="B17" s="3">
+        <v>289.10939165243286</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I17" s="3">
+        <v>188.0616</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3">
+        <f t="shared" si="0"/>
+        <v>136.12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>288.90168096607619</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I18" s="3">
+        <v>198.12</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
+        <v>147.09280000000001</v>
+      </c>
+      <c r="B19" s="3">
+        <v>288.60278919216137</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I19" s="3">
+        <v>209.09280000000001</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
+        <v>157.15120000000002</v>
+      </c>
+      <c r="B20" s="3">
+        <v>288.40339953767619</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I20" s="3">
+        <v>219.15120000000002</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>165.07600000000002</v>
+      </c>
+      <c r="B21" s="3">
+        <v>288.32007965254815</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I21" s="3">
+        <v>227.07600000000002</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>176.0488</v>
+      </c>
+      <c r="B22" s="3">
+        <v>288.22001753277391</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I22" s="3">
+        <v>238.0488</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3">
+        <f t="shared" si="0"/>
+        <v>183.9736</v>
+      </c>
+      <c r="B23" s="3">
+        <v>287.9378522251796</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I23" s="3">
+        <v>245.9736</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3">
+        <f t="shared" si="0"/>
+        <v>191.89840000000001</v>
+      </c>
+      <c r="B24" s="3">
+        <v>287.85439988132595</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I24" s="3">
+        <v>253.89840000000001</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3">
+        <f t="shared" si="0"/>
+        <v>202.87119999999999</v>
+      </c>
+      <c r="B25" s="3">
+        <v>287.65488437741692</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I25" s="3">
+        <v>264.87119999999999</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3">
+        <f t="shared" si="0"/>
+        <v>215.06319999999999</v>
+      </c>
+      <c r="B26" s="3">
+        <v>287.33938375133181</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I26" s="3">
+        <v>277.06319999999999</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3">
+        <f t="shared" si="0"/>
+        <v>227.8648</v>
+      </c>
+      <c r="B27" s="3">
+        <v>287.11477998158205</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I27" s="3">
+        <v>289.8648</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3">
+        <f t="shared" si="0"/>
+        <v>240.05680000000001</v>
+      </c>
+      <c r="B28" s="3">
+        <v>286.99766496162653</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I28" s="3">
+        <v>302.05680000000001</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3">
+        <f t="shared" si="0"/>
+        <v>252.85840000000002</v>
+      </c>
+      <c r="B29" s="3">
+        <v>286.77292748388777</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I29" s="3">
+        <v>314.85840000000002</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3">
+        <f t="shared" si="0"/>
+        <v>266.87920000000003</v>
+      </c>
+      <c r="B30" s="3">
+        <v>286.43229935657666</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I30" s="3">
+        <v>328.87920000000003</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3">
+        <f t="shared" si="0"/>
+        <v>282.11920000000003</v>
+      </c>
+      <c r="B31" s="3">
+        <v>286.19072195119617</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I31" s="3">
+        <v>344.11920000000003</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3">
+        <f t="shared" si="0"/>
+        <v>294.00640000000004</v>
+      </c>
+      <c r="B32" s="3">
+        <v>285.97425038425354</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I32" s="3">
+        <v>356.00640000000004</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3">
+        <f t="shared" si="0"/>
+        <v>307.11279999999999</v>
+      </c>
+      <c r="B33" s="3">
+        <v>285.85668796889468</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I33" s="3">
+        <v>369.11279999999999</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3">
+        <f t="shared" si="0"/>
+        <v>321.1336</v>
+      </c>
+      <c r="B34" s="3">
+        <v>285.6148763862065</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I34" s="3">
+        <v>383.1336</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3">
+        <f t="shared" si="0"/>
+        <v>333.93520000000001</v>
+      </c>
+      <c r="B35" s="3">
+        <v>285.29096603533787</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I35" s="3">
+        <v>395.93520000000001</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3">
+        <f t="shared" si="0"/>
+        <v>347.95600000000002</v>
+      </c>
+      <c r="B36" s="3">
+        <v>285.05748407224905</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I36" s="3">
+        <v>409.95600000000002</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3">
+        <f t="shared" si="0"/>
+        <v>365.02480000000003</v>
+      </c>
+      <c r="B37" s="3">
+        <v>284.69990669422975</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I37" s="3">
+        <v>427.02480000000003</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3">
+        <f t="shared" si="0"/>
+        <v>376.91200000000003</v>
+      </c>
+      <c r="B38" s="3">
+        <v>284.37604823517046</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I38" s="3">
+        <v>438.91200000000003</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3">
+        <f t="shared" si="0"/>
+        <v>392.15200000000004</v>
+      </c>
+      <c r="B39" s="3">
+        <v>284.04379501577739</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I39" s="3">
+        <v>454.15200000000004</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3">
+        <f t="shared" si="0"/>
+        <v>405.86800000000005</v>
+      </c>
+      <c r="B40" s="3">
+        <v>283.70313495285177</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I40" s="3">
+        <v>467.86800000000005</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3">
+        <f t="shared" si="0"/>
+        <v>418.06</v>
+      </c>
+      <c r="B41" s="3">
+        <v>283.38781786546514</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I41" s="3">
+        <v>480.06</v>
+      </c>
+      <c r="J41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3">
+        <f t="shared" si="0"/>
+        <v>435.12880000000001</v>
+      </c>
+      <c r="B42" s="3">
+        <v>283.22735137379397</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I42" s="3">
+        <v>497.12880000000001</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3">
+        <f t="shared" si="0"/>
+        <v>450.97840000000008</v>
+      </c>
+      <c r="B43" s="3">
+        <v>283.06666090109536</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I43" s="3">
+        <v>512.97840000000008</v>
+      </c>
+      <c r="J43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3">
+        <f t="shared" si="0"/>
+        <v>465.91359999999997</v>
+      </c>
+      <c r="B44" s="3">
+        <v>282.92269474203073</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I44" s="3">
+        <v>527.91359999999997</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3">
+        <f t="shared" si="0"/>
+        <v>479.93439999999998</v>
+      </c>
+      <c r="B45" s="3">
+        <v>282.688671638681</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I45" s="3">
+        <v>541.93439999999998</v>
+      </c>
+      <c r="J45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3">
+        <f t="shared" si="0"/>
+        <v>494.86959999999999</v>
+      </c>
+      <c r="B46" s="3">
+        <v>282.45458271673158</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I46" s="3">
+        <v>556.86959999999999</v>
+      </c>
+      <c r="J46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3">
+        <f t="shared" si="0"/>
+        <v>511.024</v>
+      </c>
+      <c r="B47" s="3">
+        <v>281.90016760549804</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I47" s="3">
+        <v>573.024</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3">
+        <f t="shared" si="0"/>
+        <v>525.95920000000001</v>
+      </c>
+      <c r="B48" s="3">
+        <v>281.75577830850921</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I48" s="3">
+        <v>587.95920000000001</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3">
+        <f t="shared" si="0"/>
+        <v>538.15120000000002</v>
+      </c>
+      <c r="B49" s="3">
+        <v>281.53856716970415</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I49" s="3">
+        <v>600.15120000000002</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3">
+        <f t="shared" si="0"/>
+        <v>554.00080000000003</v>
+      </c>
+      <c r="B50" s="3">
+        <v>281.28726766937888</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E50" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I50" s="3">
+        <v>616.00080000000003</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3">
+        <f t="shared" si="0"/>
+        <v>568.93600000000004</v>
+      </c>
+      <c r="B51" s="3">
+        <v>281.04439097290179</v>
+      </c>
+      <c r="C51" s="4">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I51" s="3">
+        <v>630.93600000000004</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3">
+        <f t="shared" si="0"/>
+        <v>585.09040000000005</v>
+      </c>
+      <c r="B52" s="3">
+        <v>280.69489455685033</v>
+      </c>
+      <c r="C52" s="4">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I52" s="3">
+        <v>647.09040000000005</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3">
+        <f t="shared" si="0"/>
+        <v>601.85440000000006</v>
+      </c>
+      <c r="B53" s="3">
+        <v>280.43482511472996</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E53" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I53" s="3">
+        <v>663.85440000000006</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3">
+        <f t="shared" si="0"/>
+        <v>615.87520000000006</v>
+      </c>
+      <c r="B54" s="3">
+        <v>280.20026972531798</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+      <c r="D54" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E54" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I54" s="3">
+        <v>677.87520000000006</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="3">
+        <f t="shared" si="0"/>
+        <v>632.94400000000007</v>
+      </c>
+      <c r="B55" s="3">
+        <v>279.93999247104853</v>
+      </c>
+      <c r="C55" s="4">
+        <v>0</v>
+      </c>
+      <c r="D55" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E55" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I55" s="3">
+        <v>694.94400000000007</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="3">
+        <f t="shared" si="0"/>
+        <v>649.09840000000008</v>
+      </c>
+      <c r="B56" s="3">
+        <v>279.59036470227318</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0</v>
+      </c>
+      <c r="D56" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E56" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I56" s="3">
+        <v>711.09840000000008</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="3">
+        <f t="shared" si="0"/>
+        <v>664.94800000000009</v>
+      </c>
+      <c r="B57" s="3">
+        <v>279.33848280551337</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0</v>
+      </c>
+      <c r="D57" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E57" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I57" s="3">
+        <v>726.94800000000009</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="3">
+        <f t="shared" si="0"/>
+        <v>679.88319999999999</v>
+      </c>
+      <c r="B58" s="3">
+        <v>279.00595685988475</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E58" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I58" s="3">
+        <v>741.88319999999999</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="3">
+        <f t="shared" si="0"/>
+        <v>696.0376</v>
+      </c>
+      <c r="B59" s="3">
+        <v>278.74536326555653</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E59" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I59" s="3">
+        <v>758.0376</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="3">
+        <f t="shared" si="0"/>
+        <v>710.05840000000001</v>
+      </c>
+      <c r="B60" s="3">
+        <v>278.51041438679204</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0</v>
+      </c>
+      <c r="D60" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E60" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I60" s="3">
+        <v>772.05840000000001</v>
+      </c>
+      <c r="J60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="3">
+        <f t="shared" si="0"/>
+        <v>727.12720000000002</v>
+      </c>
+      <c r="B61" s="3">
+        <v>278.25820411650045</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0</v>
+      </c>
+      <c r="D61" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E61" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I61" s="3">
+        <v>789.12720000000002</v>
+      </c>
+      <c r="J61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="3">
+        <f t="shared" si="0"/>
+        <v>742.97680000000003</v>
+      </c>
+      <c r="B62" s="3">
+        <v>278.00589063766995</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I62" s="3">
+        <v>804.97680000000003</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="3">
+        <f t="shared" si="0"/>
+        <v>760.04560000000004</v>
+      </c>
+      <c r="B63" s="3">
+        <v>277.74485948002638</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0</v>
+      </c>
+      <c r="D63" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E63" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I63" s="3">
+        <v>822.04560000000004</v>
+      </c>
+      <c r="J63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="3">
+        <f t="shared" si="0"/>
+        <v>774.06640000000004</v>
+      </c>
+      <c r="B64" s="3">
+        <v>277.60694608968231</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0</v>
+      </c>
+      <c r="D64" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E64" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I64" s="3">
+        <v>836.06640000000004</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="3">
+        <f t="shared" si="0"/>
+        <v>789.91600000000005</v>
+      </c>
+      <c r="B65" s="3">
+        <v>277.15963990450746</v>
+      </c>
+      <c r="C65" s="4">
+        <v>0</v>
+      </c>
+      <c r="D65" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E65" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I65" s="3">
+        <v>851.91600000000005</v>
+      </c>
+      <c r="J65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="3">
+        <f t="shared" si="0"/>
+        <v>806.98480000000006</v>
+      </c>
+      <c r="B66" s="3">
+        <v>276.90697225937356</v>
+      </c>
+      <c r="C66" s="4">
+        <v>0</v>
+      </c>
+      <c r="D66" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E66" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I66" s="3">
+        <v>868.98480000000006</v>
+      </c>
+      <c r="J66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="3">
+        <f t="shared" si="0"/>
+        <v>823.13920000000007</v>
+      </c>
+      <c r="B67" s="3">
+        <v>276.65419910732714</v>
+      </c>
+      <c r="C67" s="4">
+        <v>0</v>
+      </c>
+      <c r="D67" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E67" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I67" s="3">
+        <v>885.13920000000007</v>
+      </c>
+      <c r="J67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="3">
+        <f t="shared" si="0"/>
+        <v>838.98880000000008</v>
+      </c>
+      <c r="B68" s="3">
+        <v>276.40131995957785</v>
+      </c>
+      <c r="C68" s="4">
+        <v>0</v>
+      </c>
+      <c r="D68" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E68" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I68" s="3">
+        <v>900.98880000000008</v>
+      </c>
+      <c r="J68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="3">
+        <f t="shared" si="0"/>
+        <v>856.05760000000009</v>
+      </c>
+      <c r="B69" s="3">
+        <v>276.1483343245589</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0</v>
+      </c>
+      <c r="D69" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E69" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I69" s="3">
+        <v>918.05760000000009</v>
+      </c>
+      <c r="J69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="3">
+        <f t="shared" si="0"/>
+        <v>871.9072000000001</v>
+      </c>
+      <c r="B70" s="3">
+        <v>275.89524170790662</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0</v>
+      </c>
+      <c r="D70" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E70" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I70" s="3">
+        <v>933.9072000000001</v>
+      </c>
+      <c r="J70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="3">
+        <f t="shared" si="0"/>
+        <v>888.0616</v>
+      </c>
+      <c r="B71" s="3">
+        <v>275.83601912237026</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0</v>
+      </c>
+      <c r="D71" s="5">
+        <f t="shared" si="1"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E71" s="5">
+        <f t="shared" si="2"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I71" s="3">
+        <v>950.0616</v>
+      </c>
+      <c r="J71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="3">
+        <f t="shared" ref="A72:A135" si="3">I72-$K$1</f>
+        <v>902.99680000000001</v>
+      </c>
+      <c r="B72" s="3">
+        <v>275.5030529829549</v>
+      </c>
+      <c r="C72" s="4">
+        <v>0</v>
+      </c>
+      <c r="D72" s="5">
+        <f t="shared" ref="D72:D135" si="4">COS(RADIANS($K$5))*J72</f>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" ref="E72:E135" si="5">SIN(RADIANS($K$5))*J72</f>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I72" s="3">
+        <v>964.99680000000001</v>
+      </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="3">
+        <f t="shared" si="3"/>
+        <v>919.15120000000002</v>
+      </c>
+      <c r="B73" s="3">
+        <v>275.16141265943696</v>
+      </c>
+      <c r="C73" s="4">
+        <v>0</v>
+      </c>
+      <c r="D73" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I73" s="3">
+        <v>981.15120000000002</v>
+      </c>
+      <c r="J73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="3">
+        <f t="shared" si="3"/>
+        <v>932.86720000000003</v>
+      </c>
+      <c r="B74" s="3">
+        <v>274.92532649826245</v>
+      </c>
+      <c r="C74" s="4">
+        <v>0</v>
+      </c>
+      <c r="D74" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I74" s="3">
+        <v>994.86720000000003</v>
+      </c>
+      <c r="J74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="3">
+        <f t="shared" si="3"/>
+        <v>949.02160000000003</v>
+      </c>
+      <c r="B75" s="3">
+        <v>274.57495370993553</v>
+      </c>
+      <c r="C75" s="4">
+        <v>0</v>
+      </c>
+      <c r="D75" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I75" s="3">
+        <v>1011.0216</v>
+      </c>
+      <c r="J75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="3">
+        <f t="shared" si="3"/>
+        <v>963.95680000000016</v>
+      </c>
+      <c r="B76" s="3">
+        <v>274.25073116793152</v>
+      </c>
+      <c r="C76" s="4">
+        <v>0</v>
+      </c>
+      <c r="D76" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I76" s="3">
+        <v>1025.9568000000002</v>
+      </c>
+      <c r="J76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="3">
+        <f t="shared" si="3"/>
+        <v>980.11120000000005</v>
+      </c>
+      <c r="B77" s="3">
+        <v>274.09374224080665</v>
+      </c>
+      <c r="C77" s="4">
+        <v>0</v>
+      </c>
+      <c r="D77" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I77" s="3">
+        <v>1042.1112000000001</v>
+      </c>
+      <c r="J77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="3">
+        <f t="shared" si="3"/>
+        <v>995.96080000000006</v>
+      </c>
+      <c r="B78" s="3">
+        <v>273.83990514581308</v>
+      </c>
+      <c r="C78" s="4">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E78" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I78" s="3">
+        <v>1057.9608000000001</v>
+      </c>
+      <c r="J78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="3">
+        <f t="shared" si="3"/>
+        <v>1009.9816000000001</v>
+      </c>
+      <c r="B79" s="3">
+        <v>273.70877294220736</v>
+      </c>
+      <c r="C79" s="4">
+        <v>0</v>
+      </c>
+      <c r="D79" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E79" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I79" s="3">
+        <v>1071.9816000000001</v>
+      </c>
+      <c r="J79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="3">
+        <f t="shared" si="3"/>
+        <v>1027.0504000000001</v>
+      </c>
+      <c r="B80" s="3">
+        <v>273.35816044863839</v>
+      </c>
+      <c r="C80" s="4">
+        <v>0</v>
+      </c>
+      <c r="D80" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E80" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I80" s="3">
+        <v>1089.0504000000001</v>
+      </c>
+      <c r="J80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="3">
+        <f t="shared" si="3"/>
+        <v>1042.9000000000001</v>
+      </c>
+      <c r="B81" s="3">
+        <v>273.1040161654812</v>
+      </c>
+      <c r="C81" s="4">
+        <v>0</v>
+      </c>
+      <c r="D81" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E81" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I81" s="3">
+        <v>1104.9000000000001</v>
+      </c>
+      <c r="J81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="3">
+        <f t="shared" si="3"/>
+        <v>1056.9208000000001</v>
+      </c>
+      <c r="B82" s="3">
+        <v>272.87607276377986</v>
+      </c>
+      <c r="C82" s="4">
+        <v>0</v>
+      </c>
+      <c r="D82" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5711504387461575</v>
+      </c>
+      <c r="E82" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0641777724759121</v>
+      </c>
+      <c r="I82" s="3">
+        <v>1118.9208000000001</v>
+      </c>
+      <c r="J82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="3">
+        <f t="shared" si="3"/>
+        <v>1073.0752</v>
+      </c>
+      <c r="B83" s="3">
+        <v>273.01598967469835</v>
+      </c>
+      <c r="C83" s="4">
+        <v>0</v>
+      </c>
+      <c r="D83" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.6142172085951558</v>
+      </c>
+      <c r="E83" s="5">
+        <f t="shared" si="5"/>
+        <v>3.1155027501648838</v>
+      </c>
+      <c r="I83" s="3">
+        <v>1135.0752</v>
+      </c>
+      <c r="J83">
+        <v>4.0670000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="3">
+        <f t="shared" si="3"/>
+        <v>1090.144</v>
+      </c>
+      <c r="B84" s="3">
+        <v>273.24289001759513</v>
+      </c>
+      <c r="C84" s="4">
+        <v>0</v>
+      </c>
+      <c r="D84" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.6572839784441538</v>
+      </c>
+      <c r="E84" s="5">
+        <f t="shared" si="5"/>
+        <v>3.1668277278538555</v>
+      </c>
+      <c r="I84" s="3">
+        <v>1152.144</v>
+      </c>
+      <c r="J84">
+        <v>4.1340000000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="3">
+        <f t="shared" si="3"/>
+        <v>1105.9936</v>
+      </c>
+      <c r="B85" s="3">
+        <v>273.38169593105164</v>
+      </c>
+      <c r="C85" s="4">
+        <v>0</v>
+      </c>
+      <c r="D85" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.7003507482931517</v>
+      </c>
+      <c r="E85" s="5">
+        <f t="shared" si="5"/>
+        <v>3.2181527055428263</v>
+      </c>
+      <c r="I85" s="3">
+        <v>1167.9936</v>
+      </c>
+      <c r="J85">
+        <v>4.2009999999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="3">
+        <f t="shared" si="3"/>
+        <v>1120.0144</v>
+      </c>
+      <c r="B86" s="3">
+        <v>273.62505112710863</v>
+      </c>
+      <c r="C86" s="4">
+        <v>0</v>
+      </c>
+      <c r="D86" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.7434175181421501</v>
+      </c>
+      <c r="E86" s="5">
+        <f t="shared" si="5"/>
+        <v>3.269477683231798</v>
+      </c>
+      <c r="I86" s="3">
+        <v>1182.0144</v>
+      </c>
+      <c r="J86">
+        <v>4.2679999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="3">
+        <f t="shared" si="3"/>
+        <v>1134.9496000000001</v>
+      </c>
+      <c r="B87" s="3">
+        <v>273.78054686382507</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0</v>
+      </c>
+      <c r="D87" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.786484287991148</v>
+      </c>
+      <c r="E87" s="5">
+        <f t="shared" si="5"/>
+        <v>3.3208026609207697</v>
+      </c>
+      <c r="I87" s="3">
+        <v>1196.9496000000001</v>
+      </c>
+      <c r="J87">
+        <v>4.335</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="3">
+        <f t="shared" si="3"/>
+        <v>1151.104</v>
+      </c>
+      <c r="B88" s="3">
+        <v>273.8216870123639</v>
+      </c>
+      <c r="C88" s="4">
+        <v>0</v>
+      </c>
+      <c r="D88" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.8295510578401464</v>
+      </c>
+      <c r="E88" s="5">
+        <f t="shared" si="5"/>
+        <v>3.3721276386097414</v>
+      </c>
+      <c r="I88" s="3">
+        <v>1213.104</v>
+      </c>
+      <c r="J88">
+        <v>4.4020000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="3">
+        <f t="shared" si="3"/>
+        <v>1165.1248000000001</v>
+      </c>
+      <c r="B89" s="3">
+        <v>273.39101913996416</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0</v>
+      </c>
+      <c r="D89" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.8726178276891448</v>
+      </c>
+      <c r="E89" s="5">
+        <f t="shared" si="5"/>
+        <v>3.4234526162987131</v>
+      </c>
+      <c r="I89" s="3">
+        <v>1227.1248000000001</v>
+      </c>
+      <c r="J89">
+        <v>4.4690000000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="3">
+        <f t="shared" si="3"/>
+        <v>1180.9744000000001</v>
+      </c>
+      <c r="B90" s="3">
+        <v>273.43160651338655</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0</v>
+      </c>
+      <c r="D90" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.9156845975381422</v>
+      </c>
+      <c r="E90" s="5">
+        <f t="shared" si="5"/>
+        <v>3.4747775939876839</v>
+      </c>
+      <c r="I90" s="3">
+        <v>1242.9744000000001</v>
+      </c>
+      <c r="J90">
+        <v>4.5359999999999996</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="3">
+        <f t="shared" si="3"/>
+        <v>1198.0432000000001</v>
+      </c>
+      <c r="B91" s="3">
+        <v>273.18390899258787</v>
+      </c>
+      <c r="C91" s="4">
+        <v>0</v>
+      </c>
+      <c r="D91" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.9587513673871406</v>
+      </c>
+      <c r="E91" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5261025716766556</v>
+      </c>
+      <c r="I91" s="3">
+        <v>1260.0432000000001</v>
+      </c>
+      <c r="J91">
+        <v>4.6029999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="3">
+        <f t="shared" si="3"/>
+        <v>1213.8928000000001</v>
+      </c>
+      <c r="B92" s="3">
+        <v>272.93611060451872</v>
+      </c>
+      <c r="C92" s="4">
+        <v>0</v>
+      </c>
+      <c r="D92" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.001818137236139</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5774275493656273</v>
+      </c>
+      <c r="I92" s="3">
+        <v>1275.8928000000001</v>
+      </c>
+      <c r="J92">
+        <v>4.67</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="3">
+        <f t="shared" si="3"/>
+        <v>1227.9136000000001</v>
+      </c>
+      <c r="B93" s="3">
+        <v>272.70610382949951</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0</v>
+      </c>
+      <c r="D93" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.0448849070851369</v>
+      </c>
+      <c r="E93" s="5">
+        <f t="shared" si="5"/>
+        <v>3.6287525270545991</v>
+      </c>
+      <c r="I93" s="3">
+        <v>1289.9136000000001</v>
+      </c>
+      <c r="J93">
+        <v>4.7370000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="3">
+        <f t="shared" si="3"/>
+        <v>1247.116</v>
+      </c>
+      <c r="B94" s="3">
+        <v>272.33546107697958</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0</v>
+      </c>
+      <c r="D94" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.0879516769341353</v>
+      </c>
+      <c r="E94" s="5">
+        <f t="shared" si="5"/>
+        <v>3.6800775047435708</v>
+      </c>
+      <c r="I94" s="3">
+        <v>1309.116</v>
+      </c>
+      <c r="J94">
+        <v>4.8040000000000003</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="3">
+        <f t="shared" si="3"/>
+        <v>1262.9656</v>
+      </c>
+      <c r="B95" s="3">
+        <v>272.08740168050173</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0</v>
+      </c>
+      <c r="D95" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.1310184467831337</v>
+      </c>
+      <c r="E95" s="5">
+        <f t="shared" si="5"/>
+        <v>3.731402482432542</v>
+      </c>
+      <c r="I95" s="3">
+        <v>1324.9656</v>
+      </c>
+      <c r="J95">
+        <v>4.8710000000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="3">
+        <f t="shared" si="3"/>
+        <v>1279.1200000000001</v>
+      </c>
+      <c r="B96" s="3">
+        <v>271.83923958155373</v>
+      </c>
+      <c r="C96" s="4">
+        <v>0</v>
+      </c>
+      <c r="D96" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.1740852166321312</v>
+      </c>
+      <c r="E96" s="5">
+        <f t="shared" si="5"/>
+        <v>3.7827274601215133</v>
+      </c>
+      <c r="I96" s="3">
+        <v>1341.1200000000001</v>
+      </c>
+      <c r="J96">
+        <v>4.9379999999999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="3">
+        <f t="shared" si="3"/>
+        <v>1293.1408000000001</v>
+      </c>
+      <c r="B97" s="3">
+        <v>271.51329899978765</v>
+      </c>
+      <c r="C97" s="4">
+        <v>0</v>
+      </c>
+      <c r="D97" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.2171519864811295</v>
+      </c>
+      <c r="E97" s="5">
+        <f t="shared" si="5"/>
+        <v>3.834052437810485</v>
+      </c>
+      <c r="I97" s="3">
+        <v>1355.1408000000001</v>
+      </c>
+      <c r="J97">
+        <v>5.0049999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="3">
+        <f t="shared" si="3"/>
+        <v>1309.9048</v>
+      </c>
+      <c r="B98" s="3">
+        <v>271.0738360893796</v>
+      </c>
+      <c r="C98" s="4">
+        <v>0</v>
+      </c>
+      <c r="D98" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.2602187563301275</v>
+      </c>
+      <c r="E98" s="5">
+        <f t="shared" si="5"/>
+        <v>3.8853774154994567</v>
+      </c>
+      <c r="I98" s="3">
+        <v>1371.9048</v>
+      </c>
+      <c r="J98">
+        <v>5.0720000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="3">
+        <f t="shared" si="3"/>
+        <v>1323.9256</v>
+      </c>
+      <c r="B99" s="3">
+        <v>270.74798443998441</v>
+      </c>
+      <c r="C99" s="4">
+        <v>0</v>
+      </c>
+      <c r="D99" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.3032855261791259</v>
+      </c>
+      <c r="E99" s="5">
+        <f t="shared" si="5"/>
+        <v>3.9367023931884284</v>
+      </c>
+      <c r="I99" s="3">
+        <v>1385.9256</v>
+      </c>
+      <c r="J99">
+        <v>5.1390000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="3">
+        <f t="shared" si="3"/>
+        <v>1341.9088000000002</v>
+      </c>
+      <c r="B100" s="3">
+        <v>270.48167068549566</v>
+      </c>
+      <c r="C100" s="4">
+        <v>0</v>
+      </c>
+      <c r="D100" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.3463522960281242</v>
+      </c>
+      <c r="E100" s="5">
+        <f t="shared" si="5"/>
+        <v>3.9880273708773997</v>
+      </c>
+      <c r="I100" s="3">
+        <v>1403.9088000000002</v>
+      </c>
+      <c r="J100">
+        <v>5.2060000000000004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="3">
+        <f t="shared" si="3"/>
+        <v>1358.0632000000001</v>
+      </c>
+      <c r="B101" s="3">
+        <v>270.23322269229192</v>
+      </c>
+      <c r="C101" s="4">
+        <v>0</v>
+      </c>
+      <c r="D101" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.3894190658771217</v>
+      </c>
+      <c r="E101" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0393523485663705</v>
+      </c>
+      <c r="I101" s="3">
+        <v>1420.0632000000001</v>
+      </c>
+      <c r="J101">
+        <v>5.2729999999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="3">
+        <f t="shared" si="3"/>
+        <v>1373.9128000000001</v>
+      </c>
+      <c r="B102" s="3">
+        <v>270.27077120285315</v>
+      </c>
+      <c r="C102" s="4">
+        <v>0</v>
+      </c>
+      <c r="D102" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.4324858357261201</v>
+      </c>
+      <c r="E102" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0906773262553422</v>
+      </c>
+      <c r="I102" s="3">
+        <v>1435.9128000000001</v>
+      </c>
+      <c r="J102">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="3">
+        <f t="shared" si="3"/>
+        <v>1388.8480000000002</v>
+      </c>
+      <c r="B103" s="3">
+        <v>270.13533378576716</v>
+      </c>
+      <c r="C103" s="4">
+        <v>0</v>
+      </c>
+      <c r="D103" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.4755526055751185</v>
+      </c>
+      <c r="E103" s="5">
+        <f t="shared" si="5"/>
+        <v>4.1420023039443139</v>
+      </c>
+      <c r="I103" s="3">
+        <v>1450.8480000000002</v>
+      </c>
+      <c r="J103">
+        <v>5.407</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="3">
+        <f t="shared" si="3"/>
+        <v>1405.0024000000001</v>
+      </c>
+      <c r="B104" s="3">
+        <v>269.98163581544503</v>
+      </c>
+      <c r="C104" s="4">
+        <v>0</v>
+      </c>
+      <c r="D104" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.5186193754241164</v>
+      </c>
+      <c r="E104" s="5">
+        <f t="shared" si="5"/>
+        <v>4.1933272816332856</v>
+      </c>
+      <c r="I104" s="3">
+        <v>1467.0024000000001</v>
+      </c>
+      <c r="J104">
+        <v>5.4740000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="3">
+        <f t="shared" si="3"/>
+        <v>1420.8520000000001</v>
+      </c>
+      <c r="B105" s="3">
+        <v>269.9319961037009</v>
+      </c>
+      <c r="C105" s="4">
+        <v>0</v>
+      </c>
+      <c r="D105" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.5616861452731148</v>
+      </c>
+      <c r="E105" s="5">
+        <f t="shared" si="5"/>
+        <v>4.2446522593222573</v>
+      </c>
+      <c r="I105" s="3">
+        <v>1482.8520000000001</v>
+      </c>
+      <c r="J105">
+        <v>5.5410000000000004</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="3">
+        <f t="shared" si="3"/>
+        <v>1437.0064</v>
+      </c>
+      <c r="B106" s="3">
+        <v>269.8729843585657</v>
+      </c>
+      <c r="C106" s="4">
+        <v>0</v>
+      </c>
+      <c r="D106" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.6047529151221127</v>
+      </c>
+      <c r="E106" s="5">
+        <f t="shared" si="5"/>
+        <v>4.2959772370112281</v>
+      </c>
+      <c r="I106" s="3">
+        <v>1499.0064</v>
+      </c>
+      <c r="J106">
+        <v>5.6079999999999997</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="3">
+        <f t="shared" si="3"/>
+        <v>1454.0752</v>
+      </c>
+      <c r="B107" s="3">
+        <v>269.81364663488034</v>
+      </c>
+      <c r="C107" s="4">
+        <v>0</v>
+      </c>
+      <c r="D107" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.6478196849711106</v>
+      </c>
+      <c r="E107" s="5">
+        <f t="shared" si="5"/>
+        <v>4.3473022147001998</v>
+      </c>
+      <c r="I107" s="3">
+        <v>1516.0752</v>
+      </c>
+      <c r="J107">
+        <v>5.6749999999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="3">
+        <f t="shared" si="3"/>
+        <v>1469.9248</v>
+      </c>
+      <c r="B108" s="3">
+        <v>269.84903269887513</v>
+      </c>
+      <c r="C108" s="4">
+        <v>0</v>
+      </c>
+      <c r="D108" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.690886454820109</v>
+      </c>
+      <c r="E108" s="5">
+        <f t="shared" si="5"/>
+        <v>4.3986271923891715</v>
+      </c>
+      <c r="I108" s="3">
+        <v>1531.9248</v>
+      </c>
+      <c r="J108">
+        <v>5.742</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="3">
+        <f t="shared" si="3"/>
+        <v>1486.0792000000001</v>
+      </c>
+      <c r="B109" s="3">
+        <v>269.60811630790852</v>
+      </c>
+      <c r="C109" s="4">
+        <v>0</v>
+      </c>
+      <c r="D109" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.7339532246691074</v>
+      </c>
+      <c r="E109" s="5">
+        <f t="shared" si="5"/>
+        <v>4.4499521700781433</v>
+      </c>
+      <c r="I109" s="3">
+        <v>1548.0792000000001</v>
+      </c>
+      <c r="J109">
+        <v>5.8090000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="3">
+        <f t="shared" si="3"/>
+        <v>1501.9288000000001</v>
+      </c>
+      <c r="B110" s="3">
+        <v>269.35797636313976</v>
+      </c>
+      <c r="C110" s="4">
+        <v>0</v>
+      </c>
+      <c r="D110" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.7770199945181053</v>
+      </c>
+      <c r="E110" s="5">
+        <f t="shared" si="5"/>
+        <v>4.501277147767115</v>
+      </c>
+      <c r="I110" s="3">
+        <v>1563.9288000000001</v>
+      </c>
+      <c r="J110">
+        <v>5.8760000000000003</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="3">
+        <f t="shared" si="3"/>
+        <v>1518.9976000000001</v>
+      </c>
+      <c r="B111" s="3">
+        <v>269.10772572040588</v>
+      </c>
+      <c r="C111" s="4">
+        <v>0</v>
+      </c>
+      <c r="D111" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.8200867643671033</v>
+      </c>
+      <c r="E111" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5526021254560858</v>
+      </c>
+      <c r="I111" s="3">
+        <v>1580.9976000000001</v>
+      </c>
+      <c r="J111">
+        <v>5.9429999999999996</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="3">
+        <f t="shared" si="3"/>
+        <v>1535.152</v>
+      </c>
+      <c r="B112" s="3">
+        <v>268.86651539392102</v>
+      </c>
+      <c r="C112" s="4">
+        <v>0</v>
+      </c>
+      <c r="D112" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.8631535342161079</v>
+      </c>
+      <c r="E112" s="5">
+        <f t="shared" si="5"/>
+        <v>4.6039271031450655</v>
+      </c>
+      <c r="I112" s="3">
+        <v>1597.152</v>
+      </c>
+      <c r="J112">
+        <v>6.0100000000000096</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="3">
+        <f t="shared" si="3"/>
+        <v>1551.0016000000001</v>
+      </c>
+      <c r="B113" s="3">
+        <v>268.71083497349474</v>
+      </c>
+      <c r="C113" s="4">
+        <v>0</v>
+      </c>
+      <c r="D113" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.9062203040651058</v>
+      </c>
+      <c r="E113" s="5">
+        <f t="shared" si="5"/>
+        <v>4.6552520808340372</v>
+      </c>
+      <c r="I113" s="3">
+        <v>1613.0016000000001</v>
+      </c>
+      <c r="J113">
+        <v>6.0770000000000097</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="3">
+        <f t="shared" si="3"/>
+        <v>1566.8512000000001</v>
+      </c>
+      <c r="B114" s="3">
+        <v>268.65884085409147</v>
+      </c>
+      <c r="C114" s="4">
+        <v>0</v>
+      </c>
+      <c r="D114" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.7924468971505823</v>
+      </c>
+      <c r="E114" s="5">
+        <f t="shared" si="5"/>
+        <v>4.5196622144019702</v>
+      </c>
+      <c r="I114" s="3">
+        <v>1628.8512000000001</v>
+      </c>
+      <c r="J114">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="3">
+        <f t="shared" si="3"/>
+        <v>1583.0056000000002</v>
+      </c>
+      <c r="B115" s="3">
+        <v>268.59734985163351</v>
+      </c>
+      <c r="C115" s="4">
+        <v>0</v>
+      </c>
+      <c r="D115" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.7217402600850629</v>
+      </c>
+      <c r="E115" s="5">
+        <f t="shared" si="5"/>
+        <v>4.435397325658883</v>
+      </c>
+      <c r="I115" s="3">
+        <v>1645.0056000000002</v>
+      </c>
+      <c r="J115">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="3">
+        <f t="shared" si="3"/>
+        <v>1600.0744000000002</v>
+      </c>
+      <c r="B116" s="3">
+        <v>268.45011232359923</v>
+      </c>
+      <c r="C116" s="4">
+        <v>0</v>
+      </c>
+      <c r="D116" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.6510336230195435</v>
+      </c>
+      <c r="E116" s="5">
+        <f t="shared" si="5"/>
+        <v>4.3511324369157949</v>
+      </c>
+      <c r="I116" s="3">
+        <v>1662.0744000000002</v>
+      </c>
+      <c r="J116">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="3">
+        <f t="shared" si="3"/>
+        <v>1615.924</v>
+      </c>
+      <c r="B117" s="3">
+        <v>268.38802387474561</v>
+      </c>
+      <c r="C117" s="4">
+        <v>0</v>
+      </c>
+      <c r="D117" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.5803269859540245</v>
+      </c>
+      <c r="E117" s="5">
+        <f t="shared" si="5"/>
+        <v>4.2668675481727076</v>
+      </c>
+      <c r="I117" s="3">
+        <v>1677.924</v>
+      </c>
+      <c r="J117">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="3">
+        <f t="shared" si="3"/>
+        <v>1632.0784000000001</v>
+      </c>
+      <c r="B118" s="3">
+        <v>268.33484064928786</v>
+      </c>
+      <c r="C118" s="4">
+        <v>0</v>
+      </c>
+      <c r="D118" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.5096203488885047</v>
+      </c>
+      <c r="E118" s="5">
+        <f t="shared" si="5"/>
+        <v>4.1826026594296195</v>
+      </c>
+      <c r="I118" s="3">
+        <v>1694.0784000000001</v>
+      </c>
+      <c r="J118">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="3">
+        <f t="shared" si="3"/>
+        <v>1646.0992000000001</v>
+      </c>
+      <c r="B119" s="3">
+        <v>268.19614052573104</v>
+      </c>
+      <c r="C119" s="4">
+        <v>0</v>
+      </c>
+      <c r="D119" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.4389137118229853</v>
+      </c>
+      <c r="E119" s="5">
+        <f t="shared" si="5"/>
+        <v>4.0983377706865323</v>
+      </c>
+      <c r="I119" s="3">
+        <v>1708.0992000000001</v>
+      </c>
+      <c r="J119">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="3">
+        <f t="shared" si="3"/>
+        <v>1662.8632</v>
+      </c>
+      <c r="B120" s="3">
+        <v>268.04799895606101</v>
+      </c>
+      <c r="C120" s="4">
+        <v>0</v>
+      </c>
+      <c r="D120" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.3682070747574664</v>
+      </c>
+      <c r="E120" s="5">
+        <f t="shared" si="5"/>
+        <v>4.014072881943445</v>
+      </c>
+      <c r="I120" s="3">
+        <v>1724.8632</v>
+      </c>
+      <c r="J120">
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="3">
+        <f t="shared" si="3"/>
+        <v>1679.0176000000001</v>
+      </c>
+      <c r="B121" s="3">
+        <v>267.99401977867609</v>
+      </c>
+      <c r="C121" s="4">
+        <v>0</v>
+      </c>
+      <c r="D121" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.297500437691947</v>
+      </c>
+      <c r="E121" s="5">
+        <f t="shared" si="5"/>
+        <v>3.9298079932003573</v>
+      </c>
+      <c r="I121" s="3">
+        <v>1741.0176000000001</v>
+      </c>
+      <c r="J121">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="3">
+        <f t="shared" si="3"/>
+        <v>1694.8672000000001</v>
+      </c>
+      <c r="B122" s="3">
+        <v>267.93043621229134</v>
+      </c>
+      <c r="C122" s="4">
+        <v>0</v>
+      </c>
+      <c r="D122" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.2267938006264272</v>
+      </c>
+      <c r="E122" s="5">
+        <f t="shared" si="5"/>
+        <v>3.8455431044572692</v>
+      </c>
+      <c r="I122" s="3">
+        <v>1756.8672000000001</v>
+      </c>
+      <c r="J122">
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="3">
+        <f t="shared" si="3"/>
+        <v>1711.0216</v>
+      </c>
+      <c r="B123" s="3">
+        <v>267.87582614188977</v>
+      </c>
+      <c r="C123" s="4">
+        <v>0</v>
+      </c>
+      <c r="D123" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.1560871635609082</v>
+      </c>
+      <c r="E123" s="5">
+        <f t="shared" si="5"/>
+        <v>3.761278215714182</v>
+      </c>
+      <c r="I123" s="3">
+        <v>1773.0216</v>
+      </c>
+      <c r="J123">
+        <v>4.91</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="3">
+        <f t="shared" si="3"/>
+        <v>1728.0904</v>
+      </c>
+      <c r="B124" s="3">
+        <v>267.82090724811451</v>
+      </c>
+      <c r="C124" s="4">
+        <v>0</v>
+      </c>
+      <c r="D124" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.0853805264953889</v>
+      </c>
+      <c r="E124" s="5">
+        <f t="shared" si="5"/>
+        <v>3.6770133269710943</v>
+      </c>
+      <c r="I124" s="3">
+        <v>1790.0904</v>
+      </c>
+      <c r="J124">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="3">
+        <f t="shared" si="3"/>
+        <v>1743.94</v>
+      </c>
+      <c r="B125" s="3">
+        <v>267.67152755920716</v>
+      </c>
+      <c r="C125" s="4">
+        <v>0</v>
+      </c>
+      <c r="D125" s="5">
+        <f t="shared" si="4"/>
+        <v>-3.0146738894298699</v>
+      </c>
+      <c r="E125" s="5">
+        <f t="shared" si="5"/>
+        <v>3.592748438228007</v>
+      </c>
+      <c r="I125" s="3">
+        <v>1805.94</v>
+      </c>
+      <c r="J125">
+        <v>4.6900000000000004</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="3">
+        <f t="shared" si="3"/>
+        <v>1760.0944000000002</v>
+      </c>
+      <c r="B126" s="3">
+        <v>267.5219424943715</v>
+      </c>
+      <c r="C126" s="4">
+        <v>0</v>
+      </c>
+      <c r="D126" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.9439672523643505</v>
+      </c>
+      <c r="E126" s="5">
+        <f t="shared" si="5"/>
+        <v>3.5084835494849194</v>
+      </c>
+      <c r="I126" s="3">
+        <v>1822.0944000000002</v>
+      </c>
+      <c r="J126">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="A127" s="3">
+        <f t="shared" si="3"/>
+        <v>1776.8584000000001</v>
+      </c>
+      <c r="B127" s="3">
+        <v>267.46619715238256</v>
+      </c>
+      <c r="C127" s="4">
+        <v>0</v>
+      </c>
+      <c r="D127" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.8732606152988307</v>
+      </c>
+      <c r="E127" s="5">
+        <f t="shared" si="5"/>
+        <v>3.4242186607418317</v>
+      </c>
+      <c r="I127" s="3">
+        <v>1838.8584000000001</v>
+      </c>
+      <c r="J127">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="A128" s="3">
+        <f t="shared" si="3"/>
+        <v>1793.0128000000002</v>
+      </c>
+      <c r="B128" s="3">
+        <v>267.49474092119954</v>
+      </c>
+      <c r="C128" s="4">
+        <v>0</v>
+      </c>
+      <c r="D128" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.8025539782333118</v>
+      </c>
+      <c r="E128" s="5">
+        <f t="shared" si="5"/>
+        <v>3.3399537719987444</v>
+      </c>
+      <c r="I128" s="3">
+        <v>1855.0128000000002</v>
+      </c>
+      <c r="J128">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
+      <c r="A129" s="3">
+        <f t="shared" si="3"/>
+        <v>1808.8624000000002</v>
+      </c>
+      <c r="B129" s="3">
+        <v>267.43830100953232</v>
+      </c>
+      <c r="C129" s="4">
+        <v>0</v>
+      </c>
+      <c r="D129" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.7318473411677924</v>
+      </c>
+      <c r="E129" s="5">
+        <f t="shared" si="5"/>
+        <v>3.2556888832556568</v>
+      </c>
+      <c r="I129" s="3">
+        <v>1870.8624000000002</v>
+      </c>
+      <c r="J129">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
+      <c r="A130" s="3">
+        <f t="shared" si="3"/>
+        <v>1825.0168000000001</v>
+      </c>
+      <c r="B130" s="3">
+        <v>267.28766292162265</v>
+      </c>
+      <c r="C130" s="4">
+        <v>0</v>
+      </c>
+      <c r="D130" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.6611407041022663</v>
+      </c>
+      <c r="E130" s="5">
+        <f t="shared" si="5"/>
+        <v>3.1714239945125611</v>
+      </c>
+      <c r="I130" s="3">
+        <v>1887.0168000000001</v>
+      </c>
+      <c r="J130">
+        <v>4.1399999999999899</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
+      <c r="A131" s="3">
+        <f t="shared" si="3"/>
+        <v>1843.9144000000001</v>
+      </c>
+      <c r="B131" s="3">
+        <v>267.30559374852828</v>
+      </c>
+      <c r="C131" s="4">
+        <v>0</v>
+      </c>
+      <c r="D131" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.5904340670367469</v>
+      </c>
+      <c r="E131" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0871591057694734</v>
+      </c>
+      <c r="I131" s="3">
+        <v>1905.9144000000001</v>
+      </c>
+      <c r="J131">
+        <v>4.0299999999999896</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
+      <c r="A132" s="3">
+        <f t="shared" si="3"/>
+        <v>1860.0688</v>
+      </c>
+      <c r="B132" s="3">
+        <v>267.24817552674426</v>
+      </c>
+      <c r="C132" s="4">
+        <v>0</v>
+      </c>
+      <c r="D132" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.519727429971228</v>
+      </c>
+      <c r="E132" s="5">
+        <f t="shared" si="5"/>
+        <v>3.0028942170263861</v>
+      </c>
+      <c r="I132" s="3">
+        <v>1922.0688</v>
+      </c>
+      <c r="J132">
+        <v>3.9199999999999902</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
+      <c r="A133" s="3">
+        <f t="shared" si="3"/>
+        <v>1875.9184</v>
+      </c>
+      <c r="B133" s="3">
+        <v>267.19044022795191</v>
+      </c>
+      <c r="C133" s="4">
+        <v>0</v>
+      </c>
+      <c r="D133" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.4490207929057086</v>
+      </c>
+      <c r="E133" s="5">
+        <f t="shared" si="5"/>
+        <v>2.9186293282832985</v>
+      </c>
+      <c r="I133" s="3">
+        <v>1937.9184</v>
+      </c>
+      <c r="J133">
+        <v>3.8099999999999898</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
+      <c r="A134" s="3">
+        <f t="shared" si="3"/>
+        <v>1892.9872</v>
+      </c>
+      <c r="B134" s="3">
+        <v>267.14187885311219</v>
+      </c>
+      <c r="C134" s="4">
+        <v>0</v>
+      </c>
+      <c r="D134" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.3783141558401892</v>
+      </c>
+      <c r="E134" s="5">
+        <f t="shared" si="5"/>
+        <v>2.8343644395402108</v>
+      </c>
+      <c r="I134" s="3">
+        <v>1954.9872</v>
+      </c>
+      <c r="J134">
+        <v>3.69999999999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
+      <c r="A135" s="3">
+        <f t="shared" si="3"/>
+        <v>1909.1416000000002</v>
+      </c>
+      <c r="B135" s="3">
+        <v>266.98990825780714</v>
+      </c>
+      <c r="C135" s="4">
+        <v>0</v>
+      </c>
+      <c r="D135" s="5">
+        <f t="shared" si="4"/>
+        <v>-2.3076075187746699</v>
+      </c>
+      <c r="E135" s="5">
+        <f t="shared" si="5"/>
+        <v>2.7500995507971235</v>
+      </c>
+      <c r="I135" s="3">
+        <v>1971.1416000000002</v>
+      </c>
+      <c r="J135">
+        <v>3.5899999999999901</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
+      <c r="A136" s="3">
+        <f t="shared" ref="A136:A188" si="6">I136-$K$1</f>
+        <v>1924.9912000000002</v>
+      </c>
+      <c r="B136" s="3">
+        <v>266.83772455201921</v>
+      </c>
+      <c r="C136" s="4">
+        <v>0</v>
+      </c>
+      <c r="D136" s="5">
+        <f t="shared" ref="D136:D188" si="7">COS(RADIANS($K$5))*J136</f>
+        <v>-2.2369008817091509</v>
+      </c>
+      <c r="E136" s="5">
+        <f t="shared" ref="E136:E188" si="8">SIN(RADIANS($K$5))*J136</f>
+        <v>2.6658346620540359</v>
+      </c>
+      <c r="I136" s="3">
+        <v>1986.9912000000002</v>
+      </c>
+      <c r="J136">
+        <v>3.4799999999999902</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
+      <c r="A137" s="3">
+        <f t="shared" si="6"/>
+        <v>1942.0600000000002</v>
+      </c>
+      <c r="B137" s="3">
+        <v>266.59181883598086</v>
+      </c>
+      <c r="C137" s="4">
+        <v>0</v>
+      </c>
+      <c r="D137" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.1661942446436311</v>
+      </c>
+      <c r="E137" s="5">
+        <f t="shared" si="8"/>
+        <v>2.5815697733109482</v>
+      </c>
+      <c r="I137" s="3">
+        <v>2004.0600000000002</v>
+      </c>
+      <c r="J137">
+        <v>3.3699999999999899</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
+      <c r="A138" s="3">
+        <f t="shared" si="6"/>
+        <v>1957.9096000000002</v>
+      </c>
+      <c r="B138" s="3">
+        <v>266.53271492276764</v>
+      </c>
+      <c r="C138" s="4">
+        <v>0</v>
+      </c>
+      <c r="D138" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.0954876075781117</v>
+      </c>
+      <c r="E138" s="5">
+        <f t="shared" si="8"/>
+        <v>2.4973048845678605</v>
+      </c>
+      <c r="I138" s="3">
+        <v>2019.9096000000002</v>
+      </c>
+      <c r="J138">
+        <v>3.25999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
+      <c r="A139" s="3">
+        <f t="shared" si="6"/>
+        <v>1974.0640000000001</v>
+      </c>
+      <c r="B139" s="3">
+        <v>266.20263671062236</v>
+      </c>
+      <c r="C139" s="4">
+        <v>0</v>
+      </c>
+      <c r="D139" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.0247809705125928</v>
+      </c>
+      <c r="E139" s="5">
+        <f t="shared" si="8"/>
+        <v>2.4130399958247732</v>
+      </c>
+      <c r="I139" s="3">
+        <v>2036.0640000000001</v>
+      </c>
+      <c r="J139">
+        <v>3.1499999999999901</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
+      <c r="A140" s="3">
+        <f t="shared" si="6"/>
+        <v>1992.9616000000001</v>
+      </c>
+      <c r="B140" s="3">
+        <v>265.8438954951082</v>
+      </c>
+      <c r="C140" s="4">
+        <v>0</v>
+      </c>
+      <c r="D140" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.9540743334470732</v>
+      </c>
+      <c r="E140" s="5">
+        <f t="shared" si="8"/>
+        <v>2.3287751070816856</v>
+      </c>
+      <c r="I140" s="3">
+        <v>2054.9616000000001</v>
+      </c>
+      <c r="J140">
+        <v>3.0399999999999898</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
+      <c r="A141" s="3">
+        <f t="shared" si="6"/>
+        <v>2009.116</v>
+      </c>
+      <c r="B141" s="3">
+        <v>265.59754642696316</v>
+      </c>
+      <c r="C141" s="4">
+        <v>0</v>
+      </c>
+      <c r="D141" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.8833676963815538</v>
+      </c>
+      <c r="E141" s="5">
+        <f t="shared" si="8"/>
+        <v>2.2445102183385979</v>
+      </c>
+      <c r="I141" s="3">
+        <v>2071.116</v>
+      </c>
+      <c r="J141">
+        <v>2.9299999999999899</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
+      <c r="A142" s="3">
+        <f t="shared" si="6"/>
+        <v>2023.1368000000002</v>
+      </c>
+      <c r="B142" s="3">
+        <v>265.37024570234195</v>
+      </c>
+      <c r="C142" s="4">
+        <v>0</v>
+      </c>
+      <c r="D142" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.8126610593160346</v>
+      </c>
+      <c r="E142" s="5">
+        <f t="shared" si="8"/>
+        <v>2.1602453295955102</v>
+      </c>
+      <c r="I142" s="3">
+        <v>2085.1368000000002</v>
+      </c>
+      <c r="J142">
+        <v>2.8199999999999901</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
+      <c r="A143" s="3">
+        <f t="shared" si="6"/>
+        <v>2036.8528000000001</v>
+      </c>
+      <c r="B143" s="3">
+        <v>265.24565821699633</v>
+      </c>
+      <c r="C143" s="4">
+        <v>0</v>
+      </c>
+      <c r="D143" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.7419544222505154</v>
+      </c>
+      <c r="E143" s="5">
+        <f t="shared" si="8"/>
+        <v>2.0759804408524229</v>
+      </c>
+      <c r="I143" s="3">
+        <v>2098.8528000000001</v>
+      </c>
+      <c r="J143">
+        <v>2.7099999999999902</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
+      <c r="A144" s="3">
+        <f t="shared" si="6"/>
+        <v>2052.0927999999999</v>
+      </c>
+      <c r="B144" s="3">
+        <v>265.01817361525389</v>
+      </c>
+      <c r="C144" s="4">
+        <v>0</v>
+      </c>
+      <c r="D144" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.6712477851849958</v>
+      </c>
+      <c r="E144" s="5">
+        <f t="shared" si="8"/>
+        <v>1.991715552109335</v>
+      </c>
+      <c r="I144" s="3">
+        <v>2114.0927999999999</v>
+      </c>
+      <c r="J144">
+        <v>2.5999999999999899</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="A145" s="3">
+        <f t="shared" si="6"/>
+        <v>2067.9423999999999</v>
+      </c>
+      <c r="B145" s="3">
+        <v>264.78100904866761</v>
+      </c>
+      <c r="C145" s="4">
+        <v>0</v>
+      </c>
+      <c r="D145" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.6005411481194767</v>
+      </c>
+      <c r="E145" s="5">
+        <f t="shared" si="8"/>
+        <v>1.9074506633662476</v>
+      </c>
+      <c r="I145" s="3">
+        <v>2129.9423999999999</v>
+      </c>
+      <c r="J145">
+        <v>2.48999999999999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="A146" s="3">
+        <f t="shared" si="6"/>
+        <v>2084.0968000000003</v>
+      </c>
+      <c r="B146" s="3">
+        <v>264.53413568724852</v>
+      </c>
+      <c r="C146" s="4">
+        <v>0</v>
+      </c>
+      <c r="D146" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.5298345110539573</v>
+      </c>
+      <c r="E146" s="5">
+        <f t="shared" si="8"/>
+        <v>1.8231857746231601</v>
+      </c>
+      <c r="I146" s="3">
+        <v>2146.0968000000003</v>
+      </c>
+      <c r="J146">
+        <v>2.3799999999999901</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="A147" s="3">
+        <f t="shared" si="6"/>
+        <v>2099.9464000000003</v>
+      </c>
+      <c r="B147" s="3">
+        <v>264.38977468641667</v>
+      </c>
+      <c r="C147" s="4">
+        <v>0</v>
+      </c>
+      <c r="D147" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.4591278739884379</v>
+      </c>
+      <c r="E147" s="5">
+        <f t="shared" si="8"/>
+        <v>1.7389208858800722</v>
+      </c>
+      <c r="I147" s="3">
+        <v>2161.9464000000003</v>
+      </c>
+      <c r="J147">
+        <v>2.2699999999999898</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
+      <c r="A148" s="3">
+        <f t="shared" si="6"/>
+        <v>2114.8816000000002</v>
+      </c>
+      <c r="B148" s="3">
+        <v>264.06896396697488</v>
+      </c>
+      <c r="C148" s="4">
+        <v>0</v>
+      </c>
+      <c r="D148" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.3884212369229185</v>
+      </c>
+      <c r="E148" s="5">
+        <f t="shared" si="8"/>
+        <v>1.6546559971369847</v>
+      </c>
+      <c r="I148" s="3">
+        <v>2176.8816000000002</v>
+      </c>
+      <c r="J148">
+        <v>2.1599999999999899</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
+      <c r="A149" s="3">
+        <f t="shared" si="6"/>
+        <v>2128.9023999999999</v>
+      </c>
+      <c r="B149" s="3">
+        <v>263.93397721032653</v>
+      </c>
+      <c r="C149" s="4">
+        <v>0</v>
+      </c>
+      <c r="D149" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.3177145998573994</v>
+      </c>
+      <c r="E149" s="5">
+        <f t="shared" si="8"/>
+        <v>1.5703911083938973</v>
+      </c>
+      <c r="I149" s="3">
+        <v>2190.9023999999999</v>
+      </c>
+      <c r="J149">
+        <v>2.0499999999999901</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="A150" s="3">
+        <f t="shared" si="6"/>
+        <v>2145.0568000000003</v>
+      </c>
+      <c r="B150" s="3">
+        <v>263.69630899974669</v>
+      </c>
+      <c r="C150" s="4">
+        <v>0</v>
+      </c>
+      <c r="D150" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.24700796279188</v>
+      </c>
+      <c r="E150" s="5">
+        <f t="shared" si="8"/>
+        <v>1.4861262196508096</v>
+      </c>
+      <c r="I150" s="3">
+        <v>2207.0568000000003</v>
+      </c>
+      <c r="J150">
+        <v>1.93999999999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="A151" s="3">
+        <f t="shared" si="6"/>
+        <v>2163.9544000000001</v>
+      </c>
+      <c r="B151" s="3">
+        <v>263.43921070482281</v>
+      </c>
+      <c r="C151" s="4">
+        <v>0</v>
+      </c>
+      <c r="D151" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.1763013257263606</v>
+      </c>
+      <c r="E151" s="5">
+        <f t="shared" si="8"/>
+        <v>1.4018613309077221</v>
+      </c>
+      <c r="I151" s="3">
+        <v>2225.9544000000001</v>
+      </c>
+      <c r="J151">
+        <v>1.8299999999999901</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="A152" s="3">
+        <f t="shared" si="6"/>
+        <v>2180.1088</v>
+      </c>
+      <c r="B152" s="3">
+        <v>263.09891750702428</v>
+      </c>
+      <c r="C152" s="4">
+        <v>0</v>
+      </c>
+      <c r="D152" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.1055946886608412</v>
+      </c>
+      <c r="E152" s="5">
+        <f t="shared" si="8"/>
+        <v>1.3175964421646345</v>
+      </c>
+      <c r="I152" s="3">
+        <v>2242.1088</v>
+      </c>
+      <c r="J152">
+        <v>1.71999999999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="A153" s="3">
+        <f t="shared" si="6"/>
+        <v>2194.1296000000002</v>
+      </c>
+      <c r="B153" s="3">
+        <v>262.88035878218199</v>
+      </c>
+      <c r="C153" s="4">
+        <v>0</v>
+      </c>
+      <c r="D153" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.034888051595322</v>
+      </c>
+      <c r="E153" s="5">
+        <f t="shared" si="8"/>
+        <v>1.233331553421547</v>
+      </c>
+      <c r="I153" s="3">
+        <v>2256.1296000000002</v>
+      </c>
+      <c r="J153">
+        <v>1.6099999999999901</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
+      <c r="A154" s="3">
+        <f t="shared" si="6"/>
+        <v>2212.1128000000003</v>
+      </c>
+      <c r="B154" s="3">
+        <v>262.62296470459245</v>
+      </c>
+      <c r="C154" s="4">
+        <v>0</v>
+      </c>
+      <c r="D154" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.96418141452980266</v>
+      </c>
+      <c r="E154" s="5">
+        <f t="shared" si="8"/>
+        <v>1.1490666646784593</v>
+      </c>
+      <c r="I154" s="3">
+        <v>2274.1128000000003</v>
+      </c>
+      <c r="J154">
+        <v>1.49999999999999</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
+      <c r="A155" s="3">
+        <f t="shared" si="6"/>
+        <v>2227.9623999999999</v>
+      </c>
+      <c r="B155" s="3">
+        <v>262.18997683286347</v>
+      </c>
+      <c r="C155" s="4">
+        <v>0</v>
+      </c>
+      <c r="D155" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.89347477746428328</v>
+      </c>
+      <c r="E155" s="5">
+        <f t="shared" si="8"/>
+        <v>1.0648017759353716</v>
+      </c>
+      <c r="I155" s="3">
+        <v>2289.9623999999999</v>
+      </c>
+      <c r="J155">
+        <v>1.3899999999999899</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" s="3">
+        <f t="shared" si="6"/>
+        <v>2246.86</v>
+      </c>
+      <c r="B156" s="3">
+        <v>262.02495671996218</v>
+      </c>
+      <c r="C156" s="4">
+        <v>0</v>
+      </c>
+      <c r="D156" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.822768140398764</v>
+      </c>
+      <c r="E156" s="5">
+        <f t="shared" si="8"/>
+        <v>0.98053688719228427</v>
+      </c>
+      <c r="I156" s="3">
+        <v>2308.86</v>
+      </c>
+      <c r="J156">
+        <v>1.27999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
+      <c r="A157" s="3">
+        <f t="shared" si="6"/>
+        <v>2263.0144</v>
+      </c>
+      <c r="B157" s="3">
+        <v>261.78666666007473</v>
+      </c>
+      <c r="C157" s="4">
+        <v>0</v>
+      </c>
+      <c r="D157" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.75206150333324462</v>
+      </c>
+      <c r="E157" s="5">
+        <f t="shared" si="8"/>
+        <v>0.89627199844919658</v>
+      </c>
+      <c r="I157" s="3">
+        <v>2325.0144</v>
+      </c>
+      <c r="J157">
+        <v>1.1699999999999899</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
+      <c r="A158" s="3">
+        <f t="shared" si="6"/>
+        <v>2345.92</v>
+      </c>
+      <c r="B158" s="3">
+        <v>260.57420315644146</v>
+      </c>
+      <c r="C158" s="4">
+        <v>0</v>
+      </c>
+      <c r="D158" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.68135486626772535</v>
+      </c>
+      <c r="E158" s="5">
+        <f t="shared" si="8"/>
+        <v>0.81200710970610912</v>
+      </c>
+      <c r="I158" s="3">
+        <v>2407.92</v>
+      </c>
+      <c r="J158">
+        <v>1.0599999999999901</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
+      <c r="A159" s="3">
+        <f t="shared" si="6"/>
+        <v>2424.8632000000002</v>
+      </c>
+      <c r="B159" s="3">
+        <v>259.21445592715077</v>
+      </c>
+      <c r="C159" s="4">
+        <v>0</v>
+      </c>
+      <c r="D159" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.61064822920220596</v>
+      </c>
+      <c r="E159" s="5">
+        <f t="shared" si="8"/>
+        <v>0.72774222096302144</v>
+      </c>
+      <c r="I159" s="3">
+        <v>2486.8632000000002</v>
+      </c>
+      <c r="J159">
+        <v>0.94999999999998996</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
+      <c r="A160" s="3">
+        <f t="shared" si="6"/>
+        <v>2505.0255999999999</v>
+      </c>
+      <c r="B160" s="3">
+        <v>258.10874015104912</v>
+      </c>
+      <c r="C160" s="4">
+        <v>0</v>
+      </c>
+      <c r="D160" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.53994159213668658</v>
+      </c>
+      <c r="E160" s="5">
+        <f t="shared" si="8"/>
+        <v>0.64347733221993386</v>
+      </c>
+      <c r="I160" s="3">
+        <v>2567.0255999999999</v>
+      </c>
+      <c r="J160">
+        <v>0.83999999999998998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
+      <c r="A161" s="3">
+        <f t="shared" si="6"/>
+        <v>2591.8936000000003</v>
+      </c>
+      <c r="B161" s="3">
+        <v>256.7872773321651</v>
+      </c>
+      <c r="C161" s="4">
+        <v>0</v>
+      </c>
+      <c r="D161" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.46923495507116086</v>
+      </c>
+      <c r="E161" s="5">
+        <f t="shared" si="8"/>
+        <v>0.55921244347683863</v>
+      </c>
+      <c r="I161" s="3">
+        <v>2653.8936000000003</v>
+      </c>
+      <c r="J161">
+        <v>0.72999999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
+      <c r="A162" s="3">
+        <f t="shared" si="6"/>
+        <v>2673.8848000000003</v>
+      </c>
+      <c r="B162" s="3">
+        <v>255.4021598646606</v>
+      </c>
+      <c r="C162" s="4">
+        <v>0</v>
+      </c>
+      <c r="D162" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.3985283180056422</v>
+      </c>
+      <c r="E162" s="5">
+        <f t="shared" si="8"/>
+        <v>0.47494755473375183</v>
+      </c>
+      <c r="I162" s="3">
+        <v>2735.8848000000003</v>
+      </c>
+      <c r="J162">
+        <v>0.61999999999998101</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
+      <c r="A163" s="3">
+        <f t="shared" si="6"/>
+        <v>2751.9136000000003</v>
+      </c>
+      <c r="B163" s="3">
+        <v>254.51997480360768</v>
+      </c>
+      <c r="C163" s="4">
+        <v>0</v>
+      </c>
+      <c r="D163" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.32139380484326968</v>
+      </c>
+      <c r="E163" s="5">
+        <f t="shared" si="8"/>
+        <v>0.38302222155948901</v>
+      </c>
+      <c r="I163" s="3">
+        <v>2813.9136000000003</v>
+      </c>
+      <c r="J163">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
+      <c r="A164" s="3">
+        <f t="shared" si="6"/>
+        <v>2828.1136000000001</v>
+      </c>
+      <c r="B164" s="3">
+        <v>253.56355568755106</v>
+      </c>
+      <c r="C164" s="4">
+        <v>0</v>
+      </c>
+      <c r="D164" s="5">
+        <f t="shared" si="7"/>
+        <v>-0.69441888164700094</v>
+      </c>
+      <c r="E164" s="5">
+        <f t="shared" si="8"/>
+        <v>0.82757619696806684</v>
+      </c>
+      <c r="I164" s="3">
+        <v>2890.1136000000001</v>
+      </c>
+      <c r="J164">
+        <v>1.0803240000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
+      <c r="A165" s="3">
+        <f t="shared" si="6"/>
+        <v>2906.1424000000002</v>
+      </c>
+      <c r="B165" s="3">
+        <v>252.50349094518367</v>
+      </c>
+      <c r="C165" s="4">
+        <v>0</v>
+      </c>
+      <c r="D165" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.3557701975012872</v>
+      </c>
+      <c r="E165" s="5">
+        <f t="shared" si="8"/>
+        <v>1.6157440036043207</v>
+      </c>
+      <c r="I165" s="3">
+        <v>2968.1424000000002</v>
+      </c>
+      <c r="J165">
+        <v>2.1092039999999996</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
+      <c r="A166" s="3">
+        <f t="shared" si="6"/>
+        <v>2989.9624000000003</v>
+      </c>
+      <c r="B166" s="3">
+        <v>251.4900010972205</v>
+      </c>
+      <c r="C166" s="4">
+        <v>0</v>
+      </c>
+      <c r="D166" s="5">
+        <f t="shared" si="7"/>
+        <v>-1.8517836843920024</v>
+      </c>
+      <c r="E166" s="5">
+        <f t="shared" si="8"/>
+        <v>2.2068698585815114</v>
+      </c>
+      <c r="I166" s="3">
+        <v>3051.9624000000003</v>
+      </c>
+      <c r="J166">
+        <v>2.8808639999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
+      <c r="A167" s="3">
+        <f t="shared" si="6"/>
+        <v>3067.9911999999999</v>
+      </c>
+      <c r="B167" s="3">
+        <v>249.90502250042061</v>
+      </c>
+      <c r="C167" s="4">
+        <v>0</v>
+      </c>
+      <c r="D167" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.3808647370754321</v>
+      </c>
+      <c r="E167" s="5">
+        <f t="shared" si="8"/>
+        <v>2.8374041038905147</v>
+      </c>
+      <c r="I167" s="3">
+        <v>3129.9911999999999</v>
+      </c>
+      <c r="J167">
+        <v>3.7039680000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
+      <c r="A168" s="3">
+        <f t="shared" si="6"/>
+        <v>3145.1056000000003</v>
+      </c>
+      <c r="B168" s="3">
+        <v>249.03751767866962</v>
+      </c>
+      <c r="C168" s="4">
+        <v>0</v>
+      </c>
+      <c r="D168" s="5">
+        <f t="shared" si="7"/>
+        <v>-2.9430133555515758</v>
+      </c>
+      <c r="E168" s="5">
+        <f t="shared" si="8"/>
+        <v>3.5073467395313309</v>
+      </c>
+      <c r="I168" s="3">
+        <v>3207.1056000000003</v>
+      </c>
+      <c r="J168">
+        <v>4.5785160000000005</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
+      <c r="A169" s="3">
+        <f t="shared" si="6"/>
+        <v>3223.1344000000004</v>
+      </c>
+      <c r="B169" s="3">
+        <v>248.61328763004653</v>
+      </c>
+      <c r="C169" s="4">
+        <v>0</v>
+      </c>
+      <c r="D169" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.4059592766495763</v>
+      </c>
+      <c r="E169" s="5">
+        <f t="shared" si="8"/>
+        <v>4.0590642041767087</v>
+      </c>
+      <c r="I169" s="3">
+        <v>3285.1344000000004</v>
+      </c>
+      <c r="J169">
+        <v>5.2987320000000002</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
+      <c r="A170" s="3">
+        <f t="shared" si="6"/>
+        <v>3300.8584000000001</v>
+      </c>
+      <c r="B170" s="3">
+        <v>248.02538919714081</v>
+      </c>
+      <c r="C170" s="4">
+        <v>0</v>
+      </c>
+      <c r="D170" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.73663493457672</v>
+      </c>
+      <c r="E170" s="5">
+        <f t="shared" si="8"/>
+        <v>4.4531481074948358</v>
+      </c>
+      <c r="I170" s="3">
+        <v>3362.8584000000001</v>
+      </c>
+      <c r="J170">
+        <v>5.8131720000000007</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
+      <c r="A171" s="3">
+        <f t="shared" si="6"/>
+        <v>3384.0688</v>
+      </c>
+      <c r="B171" s="3">
+        <v>247.1130895081651</v>
+      </c>
+      <c r="C171" s="4">
+        <v>0</v>
+      </c>
+      <c r="D171" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.6043646714058624</v>
+      </c>
+      <c r="E171" s="5">
+        <f t="shared" si="8"/>
+        <v>4.2955145461675857</v>
+      </c>
+      <c r="I171" s="3">
+        <v>3446.0688</v>
+      </c>
+      <c r="J171">
+        <v>5.6073960000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
+      <c r="A172" s="3">
+        <f t="shared" si="6"/>
+        <v>3467.8888000000002</v>
+      </c>
+      <c r="B172" s="3">
+        <v>246.11841284439768</v>
+      </c>
+      <c r="C172" s="4">
+        <v>0</v>
+      </c>
+      <c r="D172" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.2736890134787187</v>
+      </c>
+      <c r="E172" s="5">
+        <f t="shared" si="8"/>
+        <v>3.9014306428494576</v>
+      </c>
+      <c r="I172" s="3">
+        <v>3529.8888000000002</v>
+      </c>
+      <c r="J172">
+        <v>5.092956</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
+      <c r="A173" s="3">
+        <f t="shared" si="6"/>
+        <v>3541.0408000000002</v>
+      </c>
+      <c r="B173" s="3">
+        <v>245.02839982230003</v>
+      </c>
+      <c r="C173" s="4">
+        <v>0</v>
+      </c>
+      <c r="D173" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.2736890134787187</v>
+      </c>
+      <c r="E173" s="5">
+        <f t="shared" si="8"/>
+        <v>3.9014306428494576</v>
+      </c>
+      <c r="I173" s="3">
+        <v>3603.0408000000002</v>
+      </c>
+      <c r="J173">
+        <v>5.092956</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
+      <c r="A174" s="3">
+        <f t="shared" si="6"/>
+        <v>3605.9632000000001</v>
+      </c>
+      <c r="B174" s="3">
+        <v>244.11016881758954</v>
+      </c>
+      <c r="C174" s="4">
+        <v>0</v>
+      </c>
+      <c r="D174" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.4059592766495763</v>
+      </c>
+      <c r="E174" s="5">
+        <f t="shared" si="8"/>
+        <v>4.0590642041767087</v>
+      </c>
+      <c r="I174" s="3">
+        <v>3667.9632000000001</v>
+      </c>
+      <c r="J174">
+        <v>5.2987320000000002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
+      <c r="A175" s="3">
+        <f t="shared" si="6"/>
+        <v>3680.0296000000003</v>
+      </c>
+      <c r="B175" s="3">
+        <v>243.12594127357258</v>
+      </c>
+      <c r="C175" s="4">
+        <v>0</v>
+      </c>
+      <c r="D175" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.4720944082350051</v>
+      </c>
+      <c r="E175" s="5">
+        <f t="shared" si="8"/>
+        <v>4.1378809848403346</v>
+      </c>
+      <c r="I175" s="3">
+        <v>3742.0296000000003</v>
+      </c>
+      <c r="J175">
+        <v>5.4016200000000003</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
+      <c r="A176" s="3">
+        <f t="shared" si="6"/>
+        <v>3765.0688</v>
+      </c>
+      <c r="B176" s="3">
+        <v>241.94382658230981</v>
+      </c>
+      <c r="C176" s="4">
+        <v>0</v>
+      </c>
+      <c r="D176" s="5">
+        <f t="shared" si="7"/>
+        <v>-3.6704998029912907</v>
+      </c>
+      <c r="E176" s="5">
+        <f t="shared" si="8"/>
+        <v>4.3743313268312098</v>
+      </c>
+      <c r="I176" s="3">
+        <v>3827.0688</v>
+      </c>
+      <c r="J176">
+        <v>5.7102839999999997</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10">
+      <c r="A177" s="3">
+        <f t="shared" si="6"/>
+        <v>3844.9264000000003</v>
+      </c>
+      <c r="B177" s="3">
+        <v>240.90050092671564</v>
+      </c>
+      <c r="C177" s="4">
+        <v>0</v>
+      </c>
+      <c r="D177" s="5">
+        <f t="shared" si="7"/>
+        <v>-4.1665132898820056</v>
+      </c>
+      <c r="E177" s="5">
+        <f t="shared" si="8"/>
+        <v>4.9654571818084001</v>
+      </c>
+      <c r="I177" s="3">
+        <v>3906.9264000000003</v>
+      </c>
+      <c r="J177">
+        <v>6.4819439999999995</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10">
+      <c r="A178" s="3">
+        <f t="shared" si="6"/>
+        <v>3914.116</v>
+      </c>
+      <c r="B178" s="3">
+        <v>239.60360805885614</v>
+      </c>
+      <c r="C178" s="4">
+        <v>0</v>
+      </c>
+      <c r="D178" s="5">
+        <f t="shared" si="7"/>
+        <v>-4.6955943425654345</v>
+      </c>
+      <c r="E178" s="5">
+        <f t="shared" si="8"/>
+        <v>5.5959914271174034</v>
+      </c>
+      <c r="I178" s="3">
+        <v>3976.116</v>
+      </c>
+      <c r="J178">
+        <v>7.3050479999999993</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10">
+      <c r="A179" s="3">
+        <f t="shared" si="6"/>
+        <v>3979.0384000000004</v>
+      </c>
+      <c r="B179" s="3">
+        <v>238.52427098962741</v>
+      </c>
+      <c r="C179" s="4">
+        <v>0</v>
+      </c>
+      <c r="D179" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.1916078294561503</v>
+      </c>
+      <c r="E179" s="5">
+        <f t="shared" si="8"/>
+        <v>6.1871172820945946</v>
+      </c>
+      <c r="I179" s="3">
+        <v>4041.0384000000004</v>
+      </c>
+      <c r="J179">
+        <v>8.076708</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
+      <c r="A180" s="3">
+        <f t="shared" si="6"/>
+        <v>4039.9984000000004</v>
+      </c>
+      <c r="B180" s="3">
+        <v>237.48804780445005</v>
+      </c>
+      <c r="C180" s="4">
+        <v>0</v>
+      </c>
+      <c r="D180" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.6545537505541512</v>
+      </c>
+      <c r="E180" s="5">
+        <f t="shared" si="8"/>
+        <v>6.7388347467399727</v>
+      </c>
+      <c r="I180" s="3">
+        <v>4101.9984000000004</v>
+      </c>
+      <c r="J180">
+        <v>8.7969240000000006</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10">
+      <c r="A181" s="3">
+        <f t="shared" si="6"/>
+        <v>4115.8936000000003</v>
+      </c>
+      <c r="B181" s="3">
+        <v>236.39479052142482</v>
+      </c>
+      <c r="C181" s="4">
+        <v>0</v>
+      </c>
+      <c r="D181" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.9190942768958648</v>
+      </c>
+      <c r="E181" s="5">
+        <f t="shared" si="8"/>
+        <v>7.0541018693944739</v>
+      </c>
+      <c r="I181" s="3">
+        <v>4177.8936000000003</v>
+      </c>
+      <c r="J181">
+        <v>9.2084759999999992</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10">
+      <c r="A182" s="3">
+        <f t="shared" si="6"/>
+        <v>4178.9872000000005</v>
+      </c>
+      <c r="B182" s="3">
+        <v>235.60505097788001</v>
+      </c>
+      <c r="C182" s="4">
+        <v>0</v>
+      </c>
+      <c r="D182" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.9852294084812945</v>
+      </c>
+      <c r="E182" s="5">
+        <f t="shared" si="8"/>
+        <v>7.1329186500581008</v>
+      </c>
+      <c r="I182" s="3">
+        <v>4240.9872000000005</v>
+      </c>
+      <c r="J182">
+        <v>9.3113640000000011</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10">
+      <c r="A183" s="3">
+        <f t="shared" si="6"/>
+        <v>4232.9368000000004</v>
+      </c>
+      <c r="B183" s="3">
+        <v>234.62155635546492</v>
+      </c>
+      <c r="C183" s="4">
+        <v>0</v>
+      </c>
+      <c r="D183" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.7868240137250089</v>
+      </c>
+      <c r="E183" s="5">
+        <f t="shared" si="8"/>
+        <v>6.8964683080672238</v>
+      </c>
+      <c r="I183" s="3">
+        <v>4294.9368000000004</v>
+      </c>
+      <c r="J183">
+        <v>9.0027000000000008</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10">
+      <c r="A184" s="3">
+        <f t="shared" si="6"/>
+        <v>4282.0096000000003</v>
+      </c>
+      <c r="B184" s="3">
+        <v>234.12385244257294</v>
+      </c>
+      <c r="C184" s="4">
+        <v>0</v>
+      </c>
+      <c r="D184" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.8529591453104359</v>
+      </c>
+      <c r="E184" s="5">
+        <f t="shared" si="8"/>
+        <v>6.975285088730848</v>
+      </c>
+      <c r="I184" s="3">
+        <v>4344.0096000000003</v>
+      </c>
+      <c r="J184">
+        <v>9.1055879999999991</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10">
+      <c r="A185" s="3">
+        <f t="shared" si="6"/>
+        <v>4331.9967999999999</v>
+      </c>
+      <c r="B185" s="3">
+        <v>233.1838801883577</v>
+      </c>
+      <c r="C185" s="4">
+        <v>0</v>
+      </c>
+      <c r="D185" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.8529591453104359</v>
+      </c>
+      <c r="E185" s="5">
+        <f t="shared" si="8"/>
+        <v>6.975285088730848</v>
+      </c>
+      <c r="I185" s="3">
+        <v>4393.9967999999999</v>
+      </c>
+      <c r="J185">
+        <v>9.1055879999999991</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10">
+      <c r="A186" s="3">
+        <f t="shared" si="6"/>
+        <v>4399.9672</v>
+      </c>
+      <c r="B186" s="3">
+        <v>232.17271729567639</v>
+      </c>
+      <c r="C186" s="4">
+        <v>0</v>
+      </c>
+      <c r="D186" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.6545537505541512</v>
+      </c>
+      <c r="E186" s="5">
+        <f t="shared" si="8"/>
+        <v>6.7388347467399727</v>
+      </c>
+      <c r="I186" s="3">
+        <v>4461.9672</v>
+      </c>
+      <c r="J186">
+        <v>8.7969240000000006</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10">
+      <c r="A187" s="3">
+        <f t="shared" si="6"/>
+        <v>4466.1088</v>
+      </c>
+      <c r="B187" s="3">
+        <v>231.27939891105586</v>
+      </c>
+      <c r="C187" s="4">
+        <v>0</v>
+      </c>
+      <c r="D187" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.5884186189687215</v>
+      </c>
+      <c r="E187" s="5">
+        <f t="shared" si="8"/>
+        <v>6.6600179660763459</v>
+      </c>
+      <c r="I187" s="3">
+        <v>4528.1088</v>
+      </c>
+      <c r="J187">
+        <v>8.6940359999999988</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10">
+      <c r="A188" s="3">
+        <f t="shared" si="6"/>
+        <v>4530.1167999999998</v>
+      </c>
+      <c r="B188" s="3">
+        <v>230.39578759028464</v>
+      </c>
+      <c r="C188" s="4">
+        <v>0</v>
+      </c>
+      <c r="D188" s="5">
+        <f t="shared" si="7"/>
+        <v>-5.9190942768958648</v>
+      </c>
+      <c r="E188" s="5">
+        <f t="shared" si="8"/>
+        <v>7.0541018693944739</v>
+      </c>
+      <c r="I188" s="3">
+        <v>4592.1167999999998</v>
+      </c>
+      <c r="J188">
+        <v>9.2084759999999992</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E193"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView showRuler="0" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3860,12 +8732,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X188"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:X188"/>
+    <sheetView showRuler="0" topLeftCell="N137" workbookViewId="0">
+      <selection activeCell="U164" sqref="U164:U188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -16571,11 +21443,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>